<commit_message>
EPBDS-12794 Explicit downcast doesn't work in arrayIndex operation
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7420_ArrayIndexOperators_Compilation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7420_ArrayIndexOperators_Compilation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED84AC1E-8615-4152-AAD7-E5A5E45EA4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE091378-1CB6-49F5-8DA3-4219F830CE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16930" yWindow="8070" windowWidth="20930" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="2970" windowWidth="16410" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Spreadsheet SpreadsheetResult transform()</t>
   </si>
@@ -34,15 +34,9 @@
     <t>S1</t>
   </si>
   <si>
-    <t xml:space="preserve">= new Object[] { 1, "2", 3.3 } </t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
-    <t>= $S1[(Number x) transform to x.doubleValue()]</t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
   <si>
@@ -52,13 +46,31 @@
     <t>S5</t>
   </si>
   <si>
-    <t>= $S1[(Number x) transform unique to x.doubleValue()]</t>
-  </si>
-  <si>
-    <t>= $S1[(Number x) split by x.doubleValue() &gt; 0]</t>
-  </si>
-  <si>
-    <t>= $S1[(Number x) select all having x.doubleValue() &gt; 0]</t>
+    <t>Datatype X</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Datatype Y</t>
+  </si>
+  <si>
+    <t>= $S1[(X x) split by x.name.length &gt; 0]</t>
+  </si>
+  <si>
+    <t>= $S1[(X x) select all having x.name.length &gt; 0]</t>
+  </si>
+  <si>
+    <t>= $S1[(X x) transform unique to x.name]</t>
+  </si>
+  <si>
+    <t>= $S1[(X x) transform to x.name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">= new Y[] { new Y("a1") } </t>
   </si>
 </sst>
 </file>
@@ -106,14 +118,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -479,16 +497,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:C14"/>
+  <dimension ref="B6:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.54296875" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.7265625" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24.26953125" style="1" customWidth="1" collapsed="1"/>
@@ -503,10 +521,10 @@
   <sheetData>
     <row r="6" spans="2:3" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -520,45 +538,75 @@
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>